<commit_message>
add test worflow, update excel for test
</commit_message>
<xml_diff>
--- a/dist/NumeroRadicacion/NumeroRadicacion.xlsx
+++ b/dist/NumeroRadicacion/NumeroRadicacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sauda\PycharmProjects\NumeroRadicacion\dist\NumeroRadicacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{576CBC11-B16A-4224-B88C-A98B0284B1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E6A89E-AEB9-4AEB-8FE7-F3654913897F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Demandante</t>
   </si>
@@ -59,13 +59,154 @@
   </si>
   <si>
     <t>18001400300120190081800.</t>
+  </si>
+  <si>
+    <t>18001400300120150044300-</t>
+  </si>
+  <si>
+    <t>18001400300320110036100.</t>
+  </si>
+  <si>
+    <t>25000234200020150182600.</t>
+  </si>
+  <si>
+    <t>05001333100520120036800.</t>
+  </si>
+  <si>
+    <t>18001400300220190085700-</t>
+  </si>
+  <si>
+    <t>18001318400120150031201-</t>
+  </si>
+  <si>
+    <t>18001311000220200026600.</t>
+  </si>
+  <si>
+    <t>18753408900120170027400.</t>
+  </si>
+  <si>
+    <t>18001333300220150092000.</t>
+  </si>
+  <si>
+    <t>18001333300120190059200.</t>
+  </si>
+  <si>
+    <t>18001400300320100008600.</t>
+  </si>
+  <si>
+    <t>18001334000320160075201.</t>
+  </si>
+  <si>
+    <t>18001400300320200033300.</t>
+  </si>
+  <si>
+    <t>18001318400320070030300.</t>
+  </si>
+  <si>
+    <t>18001333300420170059501.-</t>
+  </si>
+  <si>
+    <t>18001333300120180050701.</t>
+  </si>
+  <si>
+    <t>18001311000120190062400.-</t>
+  </si>
+  <si>
+    <t>18001333300420180052700.</t>
+  </si>
+  <si>
+    <t>18001333300120150002400.</t>
+  </si>
+  <si>
+    <t>18001333375320140005600.</t>
+  </si>
+  <si>
+    <t>18001400300220160050100.</t>
+  </si>
+  <si>
+    <t>18001400300320190053000.-</t>
+  </si>
+  <si>
+    <t>18001400300120190046100.-</t>
+  </si>
+  <si>
+    <t>18001400300420170031500.-</t>
+  </si>
+  <si>
+    <t>18001400300320170041600.-</t>
+  </si>
+  <si>
+    <t>18001400300120180055800-.</t>
+  </si>
+  <si>
+    <t>50001333300720180001500.-</t>
+  </si>
+  <si>
+    <t>18001333300220200024801.</t>
+  </si>
+  <si>
+    <t>18001333300120130083200.</t>
+  </si>
+  <si>
+    <t>18001333300120150017100.</t>
+  </si>
+  <si>
+    <t>18001400300420100033500.-</t>
+  </si>
+  <si>
+    <t>18001310300220190057400.-</t>
+  </si>
+  <si>
+    <t>18001400300420170020200.</t>
+  </si>
+  <si>
+    <t>18001310300220120046901-</t>
+  </si>
+  <si>
+    <t>18592318900120150001301.</t>
+  </si>
+  <si>
+    <t>18001311000120200032600.</t>
+  </si>
+  <si>
+    <t>18001311000220210024900.</t>
+  </si>
+  <si>
+    <t>18001311000220200024700.</t>
+  </si>
+  <si>
+    <t>18001311000220210056500.</t>
+  </si>
+  <si>
+    <t>18001311000220220004400.</t>
+  </si>
+  <si>
+    <t>18001311000220200035600 .</t>
+  </si>
+  <si>
+    <t>18001311000220220000300.</t>
+  </si>
+  <si>
+    <t>18001311000220220016000.</t>
+  </si>
+  <si>
+    <t>18001311000220220016900.</t>
+  </si>
+  <si>
+    <t>18001400300420220057800.</t>
+  </si>
+  <si>
+    <t>18001400300520220067700.</t>
+  </si>
+  <si>
+    <t>18001400300420240008600.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +219,11 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
     </font>
   </fonts>
   <fills count="3">
@@ -94,7 +240,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -117,11 +263,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -131,11 +292,20 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -186,6 +356,96 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDBFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF6600"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEC8EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike/>
         <color theme="1"/>
       </font>
@@ -498,10 +758,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -571,44 +831,309 @@
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D6" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D8" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D9" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E5" s="1"/>
+    <row r="12" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D13" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D14" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D15" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D16" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D17" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D19" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D20" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D21" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D23" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D24" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D25" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D27" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D28" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D29" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D30" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D31" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D32" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D33" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D34" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D35" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D36" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D37" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D38" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" ht="16.5" x14ac:dyDescent="0.35">
+      <c r="D39" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D40" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D41" s="6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="42" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D42" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="43" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D43" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D44" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="45" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D45" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D46" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D47" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D48" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D49" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D50" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="4:4" ht="33" x14ac:dyDescent="0.35">
+      <c r="D51" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
+  <conditionalFormatting sqref="D2:D39">
+    <cfRule type="expression" dxfId="19" priority="11">
+      <formula>$BC2="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="12">
+      <formula>$BC2="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="13">
+      <formula>$BK2="RENUNCIÉ"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="14">
+      <formula>$BC2="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="15">
+      <formula>$BA2="CURADURÍA"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>$BA2="OTRO ABOGADO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>AND($BF2="SÍ", $BI2="NO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="18">
+      <formula>AND($BI2="SÍ", $BF2="SÍ")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="19">
+      <formula>$BA2="COMPARTIDO"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="20">
+      <formula>$BA2="PARTICULAR"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D40:D51">
     <cfRule type="expression" dxfId="9" priority="1">
-      <formula>$BF2="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
+      <formula>$BC40="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="2">
-      <formula>$BF2="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
+      <formula>$BC40="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$BN2="RENUNCIÉ"</formula>
+      <formula>$BK40="RENUNCIÉ"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$BF2="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
+      <formula>$BC40="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$BD2="CURADURÍA"</formula>
+      <formula>$BA40="CURADURÍA"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$BD2="OTRO ABOGADO"</formula>
+      <formula>$BA40="OTRO ABOGADO"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="7">
-      <formula>AND($BI2="SÍ", $BL2="NO")</formula>
+      <formula>AND($BF40="SÍ", $BI40="NO")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="8">
-      <formula>AND($BL2="SÍ", $BI2="SÍ")</formula>
+      <formula>AND($BI40="SÍ", $BF40="SÍ")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="9">
-      <formula>$BD2="COMPARTIDO"</formula>
+      <formula>$BA40="COMPARTIDO"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>$BD2="PARTICULAR"</formula>
+      <formula>$BA40="PARTICULAR"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Recompile after prev change
</commit_message>
<xml_diff>
--- a/dist/NumeroRadicacion/NumeroRadicacion.xlsx
+++ b/dist/NumeroRadicacion/NumeroRadicacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sauda\PycharmProjects\NumeroRadicacion\dist\NumeroRadicacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339AF06F-B805-4C92-BF82-4D54440C7EE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDAEC5B-B036-4464-AE62-846C187568C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +186,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
         <strike/>
         <color theme="1"/>
       </font>
@@ -500,13 +498,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.08984375" bestFit="1" customWidth="1"/>
@@ -521,7 +519,7 @@
     <col min="11" max="11" width="24.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -553,7 +551,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1">
+    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -561,7 +559,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="16.5" customHeight="1">
+    <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -569,7 +567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -577,37 +575,40 @@
         <v>12</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="E5" s="1"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D4">
     <cfRule type="expression" dxfId="9" priority="1">
-      <formula>$BC2="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
+      <formula>$BF2="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="2">
-      <formula>$BC2="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
+      <formula>$BF2="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="7" priority="3">
-      <formula>$BK2="RENUNCIÉ"</formula>
+      <formula>$BN2="RENUNCIÉ"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="6" priority="4">
-      <formula>$BC2="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
+      <formula>$BF2="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="5" priority="5">
-      <formula>$BA2="CURADURÍA"</formula>
+      <formula>$BD2="CURADURÍA"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="6">
-      <formula>$BA2="OTRO ABOGADO"</formula>
+      <formula>$BD2="OTRO ABOGADO"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="7">
-      <formula>AND($BF2="SÍ", $BI2="NO")</formula>
+      <formula>AND($BI2="SÍ", $BL2="NO")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="8">
-      <formula>AND($BI2="SÍ", $BF2="SÍ")</formula>
+      <formula>AND($BL2="SÍ", $BI2="SÍ")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="9">
-      <formula>$BA2="COMPARTIDO"</formula>
+      <formula>$BD2="COMPARTIDO"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="10">
-      <formula>$BA2="PARTICULAR"</formula>
+      <formula>$BD2="PARTICULAR"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add full dist folder including _internal
</commit_message>
<xml_diff>
--- a/dist/NumeroRadicacion/NumeroRadicacion.xlsx
+++ b/dist/NumeroRadicacion/NumeroRadicacion.xlsx
@@ -1,96 +1,47 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sauda\PycharmProjects\NumeroRadicacion\dist\NumeroRadicacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EDAEC5B-B036-4464-AE62-846C187568C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Demandante</t>
-  </si>
-  <si>
-    <t>Demandado</t>
-  </si>
-  <si>
-    <t>Despacho</t>
-  </si>
-  <si>
-    <t>Radicado</t>
-  </si>
-  <si>
-    <t>Fecha de Actuacion</t>
-  </si>
-  <si>
-    <t>Actuacion</t>
-  </si>
-  <si>
-    <t>Anotacion</t>
-  </si>
-  <si>
-    <t>Fecha inicia Termino</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha finaliza Termino </t>
-  </si>
-  <si>
-    <t>Fecha de Registro</t>
-  </si>
-  <si>
-    <t>18001310500220120030203.</t>
-  </si>
-  <si>
-    <t>86001333100220170010301.</t>
-  </si>
-  <si>
-    <t>18001400300120150044300-</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.7999816888943144"/>
+        <bgColor theme="9" tint="0.7999816888943144"/>
       </patternFill>
     </fill>
   </fills>
@@ -122,13 +73,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -139,7 +90,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
+          <bgColor theme="5" tint="0.7999816888943144"/>
         </patternFill>
       </fill>
     </dxf>
@@ -152,7 +103,7 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <strike val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -162,7 +113,7 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <strike val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -180,13 +131,13 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="7" tint="0.5999633777886288"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <strike val="1"/>
         <color theme="1"/>
       </font>
       <fill>
@@ -197,7 +148,7 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <strike val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -207,7 +158,7 @@
     </dxf>
     <dxf>
       <font>
-        <strike/>
+        <strike val="1"/>
       </font>
       <fill>
         <patternFill>
@@ -224,14 +175,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -497,117 +508,578 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="79.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="255.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.08984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.08984375" bestFit="1" customWidth="1"/>
+    <col width="29.7265625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="52.08984375" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="79.54296875" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="26.7265625" bestFit="1" customWidth="1" style="1" min="4" max="4"/>
+    <col width="17" bestFit="1" customWidth="1" style="2" min="5" max="5"/>
+    <col width="27.26953125" bestFit="1" customWidth="1" style="2" min="6" max="6"/>
+    <col width="255.6328125" bestFit="1" customWidth="1" style="2" min="7" max="7"/>
+    <col width="18" bestFit="1" customWidth="1" style="2" min="8" max="8"/>
+    <col width="20.08984375" bestFit="1" customWidth="1" style="2" min="9" max="9"/>
+    <col width="15.453125" bestFit="1" customWidth="1" style="2" min="10" max="10"/>
+    <col width="24.08984375" bestFit="1" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="E5" s="1"/>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Demandante</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Demandado</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Despacho</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Radicado</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Fecha de Actuacion</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Actuacion</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Anotacion</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
+        <is>
+          <t>Fecha inicia Termino</t>
+        </is>
+      </c>
+      <c r="I1" s="2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fecha finaliza Termino </t>
+        </is>
+      </c>
+      <c r="J1" s="2" t="inlineStr">
+        <is>
+          <t>Fecha de Registro</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="16.5" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>AGUSTIN ROMERO CABEZAS</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>ORLANDO PARDO PEREZ Y MERY AZUCENA SUAREZ MORENO</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>DESPACHO 000 - TRIBUNAL SUPERIOR - CIVIL - FAMILIA - LABORAL - FLORENCIA *</t>
+        </is>
+      </c>
+      <c r="D2" s="4" t="inlineStr">
+        <is>
+          <t>18001310500220120030203.</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>2024-08-16</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Envío de expediente</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>CONFORME LO RESUELTO EN AUTO DEL 01 DE AGOSTO DEL PRESENTE AÑO, CON OFICIO REMISOIO TSSCFL-S-0250 DEL 14-08-2024, SE REMITE LASD DILIGENCIAS AL JUZGADO 02 LABORAL DEL CIRCUTIO. SE REMITE UN LINK DEL PROCESO</t>
+        </is>
+      </c>
+      <c r="H2" s="2" t="inlineStr"/>
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="inlineStr">
+        <is>
+          <t>2024-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="16.5" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>AGUEDA ROJAS DE VARGAS</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>MINISTERIO DE DEFENSA NACIONAL -EJERCITO</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>DESPACHO 000 - TRIBUNAL ADMINISTRATIVO - SIN SECCIÓN - ORAL - MOCOA *</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>86001333100220170010301.</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-02</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>DEVOLUCION ENTIDAD ORIGEN</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>MRH-Actuación automática: Proceso finalizado por: Devolucion expediente al Juzgado de origen, en cumplimiento de la Sentencia de segunda instancia de fecha 21-11-2024Devuelve al origen fecha presentación proceso: 2020-10-08, fecha providencia remisoria: 2024-12-02 Despacho origen: MARCO ANTONIO MUÑOZ MERA Tipo providencia: Sentencia - Confirma Sentencia apelada Origen: 860012333000 - MARCO ANTONIO MUÑOZ MERA Destino: 860013333002 - Juzgado Administrativo 002 ADMINISTRATIVO ORALIDAD de MOCOA (PUTUMAYO)-86001</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="inlineStr"/>
+      <c r="I3" s="2" t="inlineStr"/>
+      <c r="J3" s="2" t="inlineStr">
+        <is>
+          <t>2024-12-02</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="16.5" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>ARBEY CAMILO CANTILLO MURCIA</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>WILLIAM GERARDO HURTADO ZAPATA</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 001 CIVIL MUNICIPAL DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D4" s="4" t="inlineStr">
+        <is>
+          <t>18001400300120150044300-</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>2022-06-07</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>Archivo definitivo</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>PAQUETE 4 MARZO 2022</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr"/>
+      <c r="I4" s="2" t="inlineStr"/>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>2022-06-07</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="16.5" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>ARNULFO - ROJAS PLAZAS</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>FELIX MARIA - MONTERO POLANIA</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 003 CIVIL MUNICIPAL DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>18001400300320110036100.</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>2023-06-16</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>Fijacion estado</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>Actuación registrada el 16/06/2023 a las 14:35:50.</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>2023-06-20</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>2023-06-20</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>2023-06-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="16.5" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>BEATRIZ ZUÑIGA ARDILA</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>NACION - MINISTERIO DE DEFENSA - EJERCITO NACIONAL</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>DESPACHO 000 - TRIBUNAL ADMINISTRATIVO - SECCIÓN SEGUNDA MIXTA - ORAL - BOGOTÁ *</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="inlineStr">
+        <is>
+          <t>25000234200020150182600.</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>2022-02-08</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>ARCHIVO</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>43710</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr"/>
+      <c r="I6" s="2" t="inlineStr"/>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>2022-02-08</t>
+        </is>
+      </c>
+    </row>
+    <row r="7" ht="16.5" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>FELIX CONEO MUÑOZ</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>NACION-MINDEFENSA-POLICIA</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 031 ADMINISTRATIVO DE MEDELLÍN</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
+        <is>
+          <t>05001333100520120036800.</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>2017-10-12</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>Archivo</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>CAJA 9848</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>2017-10-12</t>
+        </is>
+      </c>
+      <c r="K7" s="1" t="n"/>
+    </row>
+    <row r="8" ht="16.5" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>CAROL OSORNO CARDONA</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>LAURA MARIA ROJAS RIVERA</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 002 CIVIL MUNICIPAL DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D8" s="4" t="inlineStr">
+        <is>
+          <t>18001400300220190085700-</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>2024-08-20</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>Entrega de oficios</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="inlineStr">
+        <is>
+          <t>Constancia Notificacion del los Oficios No. 1669 y 1670 a Bancos - Levanta Medidas.</t>
+        </is>
+      </c>
+      <c r="H8" s="2" t="inlineStr"/>
+      <c r="I8" s="2" t="inlineStr"/>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>2024-08-30</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="16.5" customHeight="1">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>CARLOS EDUARDO- HURTADO SUZUNAGA</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>CAUSANTE OSCAR REINALDO - HURTADO MUÑOZ</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 001 DE FAMILIA DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="inlineStr">
+        <is>
+          <t>18001318400120150031201-</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>Fijacion estado</t>
+        </is>
+      </c>
+      <c r="G9" s="2" t="inlineStr">
+        <is>
+          <t>Actuación registrada el 20/05/2024 a las 12:00:21.</t>
+        </is>
+      </c>
+      <c r="H9" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="I9" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-21</t>
+        </is>
+      </c>
+      <c r="J9" s="2" t="inlineStr">
+        <is>
+          <t>2024-05-20</t>
+        </is>
+      </c>
+    </row>
+    <row r="10" ht="16.5" customHeight="1">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>DANIELA - ROJAS CUÉLLAR</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr"/>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 002 DE FAMILIA DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D10" s="4" t="inlineStr">
+        <is>
+          <t>18001311000220200026600.</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>2021-04-16</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>Fijacion estado</t>
+        </is>
+      </c>
+      <c r="G10" s="2" t="inlineStr">
+        <is>
+          <t>Actuación registrada el 16/04/2021 a las 11:04:55.</t>
+        </is>
+      </c>
+      <c r="H10" s="2" t="inlineStr">
+        <is>
+          <t>2021-04-19</t>
+        </is>
+      </c>
+      <c r="I10" s="2" t="inlineStr">
+        <is>
+          <t>2021-04-19</t>
+        </is>
+      </c>
+      <c r="J10" s="2" t="inlineStr">
+        <is>
+          <t>2021-04-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="11" ht="16.5" customHeight="1">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>WILMAR ARTUNDUAGA ALVAREZ</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>DIANA PATRICIA MORERA SANCHEZ</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>JUZGADO 001 CIVIL MUNICIPAL DE FLORENCIA</t>
+        </is>
+      </c>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>18001400300120190081800.</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>2021-10-14</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>Archivo definitivo</t>
+        </is>
+      </c>
+      <c r="G11" s="2" t="inlineStr">
+        <is>
+          <t>PAQUETE 2 JUNIO 2021</t>
+        </is>
+      </c>
+      <c r="H11" s="2" t="inlineStr"/>
+      <c r="I11" s="2" t="inlineStr"/>
+      <c r="J11" s="2" t="inlineStr">
+        <is>
+          <t>2021-10-14</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="E12" s="1" t="n"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:D4">
-    <cfRule type="expression" dxfId="9" priority="1">
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="expression" priority="1" dxfId="9">
       <formula>$BF2="FINALIZADO POR EXTINCIÓN DE LA ACCIÓN DISCIPLINARIA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="2">
+    <cfRule type="expression" priority="2" dxfId="7">
       <formula>$BF2="FINALIZADO POR SENTENCIA QUE NIEGA PRETENSIONES"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" priority="3" dxfId="7">
       <formula>$BN2="RENUNCIÉ"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" priority="4" dxfId="6">
       <formula>$BF2="FINALIZADO POR SENTENCIA QUE CONCEDE PRETENSIONES"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" priority="5" dxfId="5">
       <formula>$BD2="CURADURÍA"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
+    <cfRule type="expression" priority="6" dxfId="4">
       <formula>$BD2="OTRO ABOGADO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="7">
+    <cfRule type="expression" priority="7" dxfId="3">
       <formula>AND($BI2="SÍ", $BL2="NO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="8">
+    <cfRule type="expression" priority="8" dxfId="2">
       <formula>AND($BL2="SÍ", $BI2="SÍ")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="9">
+    <cfRule type="expression" priority="9" dxfId="1">
       <formula>$BD2="COMPARTIDO"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" priority="10" dxfId="0">
       <formula>$BD2="PARTICULAR"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>